<commit_message>
Fixed valuation model for BENDIGO.xlsx
</commit_message>
<xml_diff>
--- a/Assignment/BENDIGO.xlsx
+++ b/Assignment/BENDIGO.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua Stamatellos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh\Documents\GITHUB\FM_equity_research\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10020001_{80537A58-7129-47F6-8090-2DF96F4420DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FB68F1-9F55-437C-9375-61BE8DE2E6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C40C285E-7926-4BFA-A8EA-1C74888DBDA3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C40C285E-7926-4BFA-A8EA-1C74888DBDA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dividend Discount Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -378,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -428,19 +427,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -793,34 +790,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314E70D6-0A07-40D1-BF88-F5CE50014335}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="82" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="1.7265625" customWidth="1"/>
+    <col min="2" max="2" width="2.7265625" customWidth="1"/>
+    <col min="3" max="3" width="3.1796875" customWidth="1"/>
+    <col min="4" max="4" width="44.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="7" max="9" width="9.1796875" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="10" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2"/>
       <c r="B2" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.4">
       <c r="A3"/>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -857,7 +856,7 @@
         <v>46935</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -894,7 +893,7 @@
         <v>47299</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -925,10 +924,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="31" t="s">
@@ -941,7 +940,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="45">
+      <c r="J9" s="44">
         <v>45772</v>
       </c>
       <c r="K9" s="6"/>
@@ -954,7 +953,7 @@
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="31" t="s">
@@ -967,7 +966,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="46">
+      <c r="J10" s="45">
         <v>10.88</v>
       </c>
       <c r="K10" s="6"/>
@@ -980,8 +979,7 @@
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
     </row>
-    <row r="11" spans="1:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11"/>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="31" t="s">
@@ -994,7 +992,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="43">
+      <c r="J11" s="42">
         <v>566.54</v>
       </c>
       <c r="K11" s="6"/>
@@ -1007,7 +1005,7 @@
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="31" t="s">
@@ -1020,7 +1018,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="47">
+      <c r="J12" s="46">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="K12" s="6"/>
@@ -1033,7 +1031,7 @@
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="31" t="s">
@@ -1046,7 +1044,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="47">
+      <c r="J13" s="46">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="K13" s="6"/>
@@ -1059,7 +1057,7 @@
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1073,24 +1071,24 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15"/>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1104,7 +1102,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
@@ -1123,7 +1121,7 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
@@ -1131,7 +1129,7 @@
       </c>
       <c r="E18" s="34">
         <f>J49</f>
-        <v>10.921636606380696</v>
+        <v>13.891761642724171</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1142,15 +1140,15 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="55">
+      <c r="E19" s="53">
         <f>E18/E17-1</f>
-        <v>3.8268939688139714E-3</v>
+        <v>0.27681632745626561</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -1161,7 +1159,7 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -1175,30 +1173,30 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21"/>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
-      <c r="S21" s="41"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1218,7 +1216,7 @@
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
     </row>
-    <row r="23" spans="1:19" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
@@ -1241,7 +1239,7 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B24" s="11"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1261,7 +1259,7 @@
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
       <c r="D25" s="6" t="s">
@@ -1275,19 +1273,19 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="44">
+      <c r="K25" s="43">
         <f>$J$11</f>
         <v>566.54</v>
       </c>
-      <c r="L25" s="44">
+      <c r="L25" s="43">
         <f t="shared" ref="L25:M25" si="0">$J$11</f>
         <v>566.54</v>
       </c>
-      <c r="M25" s="44">
+      <c r="M25" s="43">
         <f t="shared" si="0"/>
         <v>566.54</v>
       </c>
-      <c r="N25" s="48">
+      <c r="N25" s="47">
         <f>M25</f>
         <v>566.54</v>
       </c>
@@ -1309,7 +1307,7 @@
       </c>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
       <c r="D26" s="6" t="s">
@@ -1323,33 +1321,33 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="17"/>
-      <c r="K26" s="43">
+      <c r="K26" s="42">
         <v>488.1</v>
       </c>
-      <c r="L26" s="43">
+      <c r="L26" s="42">
         <v>497</v>
       </c>
-      <c r="M26" s="42">
+      <c r="M26" s="41">
         <v>545</v>
       </c>
-      <c r="N26" s="43">
+      <c r="N26" s="42">
         <v>455.86</v>
       </c>
-      <c r="O26" s="43">
+      <c r="O26" s="42">
         <v>491.76</v>
       </c>
-      <c r="P26" s="43">
+      <c r="P26" s="42">
         <v>500.55</v>
       </c>
-      <c r="Q26" s="43">
+      <c r="Q26" s="42">
         <v>515.5</v>
       </c>
-      <c r="R26" s="43">
+      <c r="R26" s="42">
         <v>611</v>
       </c>
       <c r="S26" s="7"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B27" s="11"/>
       <c r="C27" s="7"/>
       <c r="D27" s="6" t="s">
@@ -1367,7 +1365,7 @@
         <f>K25*K31</f>
         <v>300.26619999999997</v>
       </c>
-      <c r="L27" s="51">
+      <c r="L27" s="17">
         <f t="shared" ref="L27:M27" si="1">L25*L31</f>
         <v>345.58939999999996</v>
       </c>
@@ -1375,29 +1373,29 @@
         <f t="shared" si="1"/>
         <v>356.92019999999997</v>
       </c>
-      <c r="N27" s="51">
+      <c r="N27" s="17">
         <f>N31*N25</f>
         <v>298.65271073691014</v>
       </c>
-      <c r="O27" s="51">
+      <c r="O27" s="17">
         <f t="shared" ref="O27:R27" si="2">O31*O25</f>
         <v>322.17228322726919</v>
       </c>
-      <c r="P27" s="51">
+      <c r="P27" s="17">
         <f t="shared" si="2"/>
         <v>327.93097521028471</v>
       </c>
-      <c r="Q27" s="51">
+      <c r="Q27" s="17">
         <f t="shared" si="2"/>
         <v>337.72533757047592</v>
       </c>
-      <c r="R27" s="51">
+      <c r="R27" s="17">
         <f t="shared" si="2"/>
         <v>400.29133124260096</v>
       </c>
       <c r="S27" s="7"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B28" s="11"/>
       <c r="C28" s="7"/>
       <c r="D28" s="6"/>
@@ -1417,7 +1415,7 @@
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6" t="s">
@@ -1465,7 +1463,7 @@
       </c>
       <c r="S29" s="6"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6" t="s">
@@ -1479,41 +1477,41 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="20"/>
-      <c r="K30" s="52">
+      <c r="K30" s="50">
         <f>K27/K26</f>
         <v>0.61517353001434127</v>
       </c>
-      <c r="L30" s="52">
-        <f t="shared" ref="L30:R30" si="4">L27/L26</f>
+      <c r="L30" s="50">
+        <f t="shared" ref="L30:M30" si="4">L27/L26</f>
         <v>0.69535090543259548</v>
       </c>
-      <c r="M30" s="53">
+      <c r="M30" s="51">
         <f t="shared" si="4"/>
         <v>0.65489944954128432</v>
       </c>
-      <c r="N30" s="52">
+      <c r="N30" s="50">
         <f>AVERAGE($K$30:$M$30)</f>
         <v>0.65514129499607365</v>
       </c>
-      <c r="O30" s="52">
+      <c r="O30" s="50">
         <f t="shared" ref="O30:R30" si="5">AVERAGE($K$30:$M$30)</f>
         <v>0.65514129499607365</v>
       </c>
-      <c r="P30" s="52">
+      <c r="P30" s="50">
         <f t="shared" si="5"/>
         <v>0.65514129499607365</v>
       </c>
-      <c r="Q30" s="52">
+      <c r="Q30" s="50">
         <f t="shared" si="5"/>
         <v>0.65514129499607365</v>
       </c>
-      <c r="R30" s="52">
+      <c r="R30" s="50">
         <f t="shared" si="5"/>
         <v>0.65514129499607365</v>
       </c>
       <c r="S30" s="6"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
@@ -1527,13 +1525,13 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="20"/>
-      <c r="K31" s="49">
+      <c r="K31" s="48">
         <v>0.53</v>
       </c>
-      <c r="L31" s="49">
+      <c r="L31" s="48">
         <v>0.61</v>
       </c>
-      <c r="M31" s="50">
+      <c r="M31" s="49">
         <v>0.63</v>
       </c>
       <c r="N31" s="22">
@@ -1558,7 +1556,7 @@
       </c>
       <c r="S31" s="6"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -1578,7 +1576,7 @@
       <c r="R32" s="6"/>
       <c r="S32" s="6"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
@@ -1617,7 +1615,7 @@
       </c>
       <c r="S33" s="6"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6" t="s">
@@ -1656,7 +1654,7 @@
       </c>
       <c r="S34" s="6"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="25" t="s">
@@ -1695,7 +1693,7 @@
       </c>
       <c r="S35" s="27"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -1715,7 +1713,7 @@
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="31" t="s">
@@ -1742,7 +1740,7 @@
       <c r="R37" s="6"/>
       <c r="S37" s="6"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -1762,7 +1760,7 @@
       <c r="R38" s="6"/>
       <c r="S38" s="6"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -1782,7 +1780,7 @@
       <c r="R39" s="6"/>
       <c r="S39" s="6"/>
     </row>
-    <row r="40" spans="1:19" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40"/>
       <c r="B40" s="6"/>
       <c r="C40" s="8" t="s">
@@ -1805,7 +1803,7 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -1825,7 +1823,7 @@
       <c r="R41" s="6"/>
       <c r="S41" s="6"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6" t="s">
@@ -1852,7 +1850,7 @@
       <c r="R42" s="6"/>
       <c r="S42" s="6"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6" t="s">
@@ -1879,7 +1877,7 @@
       <c r="R43" s="6"/>
       <c r="S43" s="6"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6" t="s">
@@ -1906,7 +1904,7 @@
       <c r="R44" s="6"/>
       <c r="S44" s="6"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6" t="s">
@@ -1933,7 +1931,7 @@
       <c r="R45" s="6"/>
       <c r="S45" s="6"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6" t="s">
@@ -1960,7 +1958,7 @@
       <c r="R46" s="6"/>
       <c r="S46" s="6"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="27" t="s">
@@ -1987,7 +1985,7 @@
       <c r="R47" s="6"/>
       <c r="S47" s="6"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6" t="s">
@@ -2001,8 +1999,8 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="34">
-        <f>$J$40</f>
-        <v>0</v>
+        <f>$J$37</f>
+        <v>2.9701250363434752</v>
       </c>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
@@ -2014,7 +2012,7 @@
       <c r="R48" s="6"/>
       <c r="S48" s="6"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="25" t="s">
@@ -2029,7 +2027,7 @@
       <c r="I49" s="27"/>
       <c r="J49" s="36">
         <f>SUM(J47:J48)</f>
-        <v>10.921636606380696</v>
+        <v>13.891761642724171</v>
       </c>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
@@ -2041,28 +2039,28 @@
       <c r="R49" s="6"/>
       <c r="S49" s="6"/>
     </row>
-    <row r="51" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51"/>
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="41"/>
-      <c r="L51" s="41"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="41"/>
-      <c r="O51" s="41"/>
-      <c r="P51" s="41"/>
-      <c r="Q51" s="41"/>
-      <c r="R51" s="41"/>
-      <c r="S51" s="41"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="40"/>
+      <c r="M51" s="40"/>
+      <c r="N51" s="40"/>
+      <c r="O51" s="40"/>
+      <c r="P51" s="40"/>
+      <c r="Q51" s="40"/>
+      <c r="R51" s="40"/>
+      <c r="S51" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Table in right column
</commit_message>
<xml_diff>
--- a/Assignment/BENDIGO.xlsx
+++ b/Assignment/BENDIGO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh\Documents\GITHUB\FM_equity_research\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FB68F1-9F55-437C-9375-61BE8DE2E6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A578B6-2DD4-4E88-BF30-5836CC113263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C40C285E-7926-4BFA-A8EA-1C74888DBDA3}"/>
   </bookViews>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314E70D6-0A07-40D1-BF88-F5CE50014335}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="82" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,26 +800,26 @@
     <col min="2" max="2" width="2.7265625" customWidth="1"/>
     <col min="3" max="3" width="3.1796875" customWidth="1"/>
     <col min="4" max="4" width="44.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
     <col min="7" max="9" width="9.1796875" customWidth="1"/>
     <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="18" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="10" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" ht="10" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2"/>
       <c r="B2" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.4">
       <c r="A3"/>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -856,7 +856,7 @@
         <v>46935</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -893,7 +893,7 @@
         <v>47299</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -924,10 +924,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="31" t="s">
@@ -936,24 +936,20 @@
       <c r="E9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="44">
+        <v>45772</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="44">
-        <v>45772</v>
-      </c>
+      <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="31" t="s">
@@ -962,24 +958,20 @@
       <c r="E10" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="45">
+        <v>10.88</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="45">
-        <v>10.88</v>
-      </c>
+      <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="31" t="s">
@@ -988,24 +980,20 @@
       <c r="E11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="42">
+        <v>566.54</v>
+      </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="42">
-        <v>566.54</v>
-      </c>
+      <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="38"/>
+      <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="31" t="s">
@@ -1014,24 +1002,20 @@
       <c r="E12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="46">
+        <v>7.9000000000000001E-2</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="46">
-        <v>7.9000000000000001E-2</v>
-      </c>
+      <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="31" t="s">
@@ -1040,24 +1024,20 @@
       <c r="E13" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="46">
+        <v>2.1000000000000001E-2</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="46">
-        <v>2.1000000000000001E-2</v>
-      </c>
+      <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1071,7 +1051,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15" s="39" t="s">
         <v>41</v>
@@ -1088,7 +1068,7 @@
       <c r="L15" s="52"/>
       <c r="M15" s="52"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1109,7 +1089,7 @@
         <v>35</v>
       </c>
       <c r="E17" s="22">
-        <f>J10</f>
+        <f>F10</f>
         <v>10.88</v>
       </c>
       <c r="F17" s="6"/>
@@ -1128,7 +1108,7 @@
         <v>42</v>
       </c>
       <c r="E18" s="34">
-        <f>J49</f>
+        <f>F49</f>
         <v>13.891761642724171</v>
       </c>
       <c r="F18" s="6"/>
@@ -1274,15 +1254,15 @@
       <c r="I25" s="7"/>
       <c r="J25" s="14"/>
       <c r="K25" s="43">
-        <f>$J$11</f>
+        <f>$F$11</f>
         <v>566.54</v>
       </c>
       <c r="L25" s="43">
-        <f t="shared" ref="L25:M25" si="0">$J$11</f>
+        <f>$F$11</f>
         <v>566.54</v>
       </c>
       <c r="M25" s="43">
-        <f t="shared" si="0"/>
+        <f>$F$11</f>
         <v>566.54</v>
       </c>
       <c r="N25" s="47">
@@ -1366,11 +1346,11 @@
         <v>300.26619999999997</v>
       </c>
       <c r="L27" s="17">
-        <f t="shared" ref="L27:M27" si="1">L25*L31</f>
+        <f t="shared" ref="L27:M27" si="0">L25*L31</f>
         <v>345.58939999999996</v>
       </c>
       <c r="M27" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>356.92019999999997</v>
       </c>
       <c r="N27" s="17">
@@ -1378,19 +1358,19 @@
         <v>298.65271073691014</v>
       </c>
       <c r="O27" s="17">
-        <f t="shared" ref="O27:R27" si="2">O31*O25</f>
+        <f t="shared" ref="O27:R27" si="1">O31*O25</f>
         <v>322.17228322726919</v>
       </c>
       <c r="P27" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>327.93097521028471</v>
       </c>
       <c r="Q27" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>337.72533757047592</v>
       </c>
       <c r="R27" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>400.29133124260096</v>
       </c>
       <c r="S27" s="7"/>
@@ -1430,15 +1410,15 @@
       <c r="I29" s="6"/>
       <c r="J29" s="20"/>
       <c r="K29" s="20">
-        <f t="shared" ref="K29:R29" si="3">K26/K25</f>
+        <f t="shared" ref="K29:R29" si="2">K26/K25</f>
         <v>0.86154552194019851</v>
       </c>
       <c r="L29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.87725491580470938</v>
       </c>
       <c r="M29" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.9619797366470153</v>
       </c>
       <c r="N29" s="20">
@@ -1446,19 +1426,19 @@
         <v>0.80463868394111637</v>
       </c>
       <c r="O29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.86800578952942431</v>
       </c>
       <c r="P29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.88352102234617158</v>
       </c>
       <c r="Q29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.90990927383768139</v>
       </c>
       <c r="R29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.0784763653051859</v>
       </c>
       <c r="S29" s="6"/>
@@ -1482,11 +1462,11 @@
         <v>0.61517353001434127</v>
       </c>
       <c r="L30" s="50">
-        <f t="shared" ref="L30:M30" si="4">L27/L26</f>
+        <f t="shared" ref="L30:M30" si="3">L27/L26</f>
         <v>0.69535090543259548</v>
       </c>
       <c r="M30" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.65489944954128432</v>
       </c>
       <c r="N30" s="50">
@@ -1494,19 +1474,19 @@
         <v>0.65514129499607365</v>
       </c>
       <c r="O30" s="50">
-        <f t="shared" ref="O30:R30" si="5">AVERAGE($K$30:$M$30)</f>
+        <f t="shared" ref="O30:R30" si="4">AVERAGE($K$30:$M$30)</f>
         <v>0.65514129499607365</v>
       </c>
       <c r="P30" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.65514129499607365</v>
       </c>
       <c r="Q30" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.65514129499607365</v>
       </c>
       <c r="R30" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.65514129499607365</v>
       </c>
       <c r="S30" s="6"/>
@@ -1539,19 +1519,19 @@
         <v>0.52715202940111938</v>
       </c>
       <c r="O31" s="22">
-        <f t="shared" ref="O31:R31" si="6">O30*O29</f>
+        <f t="shared" ref="O31:R31" si="5">O30*O29</f>
         <v>0.56866643701639641</v>
       </c>
       <c r="P31" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.57883110673612581</v>
       </c>
       <c r="Q31" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.59611913999095556</v>
       </c>
       <c r="R31" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.70655440258869806</v>
       </c>
       <c r="S31" s="6"/>
@@ -1598,19 +1578,19 @@
         <v>45838</v>
       </c>
       <c r="O33" s="23">
-        <f t="shared" ref="O33:R33" si="7">O5</f>
+        <f t="shared" ref="O33:R33" si="6">O5</f>
         <v>46203</v>
       </c>
       <c r="P33" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>46568</v>
       </c>
       <c r="Q33" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>46934</v>
       </c>
       <c r="R33" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>47299</v>
       </c>
       <c r="S33" s="6"/>
@@ -1633,23 +1613,23 @@
       <c r="L34" s="18"/>
       <c r="M34" s="19"/>
       <c r="N34" s="22">
-        <f>(N33-$J$9)/365</f>
+        <f>(N33-$F$9)/365</f>
         <v>0.18082191780821918</v>
       </c>
       <c r="O34" s="22">
-        <f t="shared" ref="O34:R34" si="8">(O33-$J$9)/365</f>
+        <f t="shared" ref="O34:R34" si="7">(O33-$F$9)/365</f>
         <v>1.1808219178082191</v>
       </c>
       <c r="P34" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.1808219178082191</v>
       </c>
       <c r="Q34" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.1835616438356165</v>
       </c>
       <c r="R34" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>4.183561643835616</v>
       </c>
       <c r="S34" s="6"/>
@@ -1672,23 +1652,23 @@
       <c r="L35" s="28"/>
       <c r="M35" s="29"/>
       <c r="N35" s="30">
-        <f>N31/(1+J12)^N34</f>
+        <f>N31/(1+F12)^N34</f>
         <v>0.51995395001129951</v>
       </c>
       <c r="O35" s="30">
-        <f t="shared" ref="O35:R35" si="9">O31/(1+K12)^O34</f>
+        <f>O31/(1+G12)^O34</f>
         <v>0.56866643701639641</v>
       </c>
       <c r="P35" s="30">
-        <f t="shared" si="9"/>
+        <f>P31/(1+H12)^P34</f>
         <v>0.57883110673612581</v>
       </c>
       <c r="Q35" s="30">
-        <f t="shared" si="9"/>
+        <f>Q31/(1+I12)^Q34</f>
         <v>0.59611913999095556</v>
       </c>
       <c r="R35" s="30">
-        <f t="shared" si="9"/>
+        <f>R31/(1+J12)^R34</f>
         <v>0.70655440258869806</v>
       </c>
       <c r="S35" s="27"/>
@@ -1832,23 +1812,19 @@
       <c r="E42" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F42" s="6"/>
+      <c r="F42" s="34">
+        <f>R31</f>
+        <v>0.70655440258869806</v>
+      </c>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
-      <c r="J42" s="34">
-        <f>R31</f>
-        <v>0.70655440258869806</v>
-      </c>
+      <c r="J42" s="6"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B43" s="6"/>
@@ -1859,23 +1835,19 @@
       <c r="E43" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="6"/>
+      <c r="F43" s="35">
+        <f>F13</f>
+        <v>2.1000000000000001E-2</v>
+      </c>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
-      <c r="J43" s="35">
-        <f>J13</f>
-        <v>2.1000000000000001E-2</v>
-      </c>
+      <c r="J43" s="6"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="6"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B44" s="6"/>
@@ -1886,23 +1858,19 @@
       <c r="E44" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="6"/>
+      <c r="F44" s="34">
+        <f>F42*(1+F43)</f>
+        <v>0.72139204504306065</v>
+      </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
-      <c r="J44" s="34">
-        <f>J42*(1+J43)</f>
-        <v>0.72139204504306065</v>
-      </c>
+      <c r="J44" s="6"/>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="6"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B45" s="6"/>
@@ -1913,23 +1881,19 @@
       <c r="E45" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F45" s="6"/>
+      <c r="F45" s="34">
+        <f>F44/(F12-F43)</f>
+        <v>12.437793880052771</v>
+      </c>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-      <c r="J45" s="34">
-        <f>J44/(J12-J43)</f>
-        <v>12.437793880052771</v>
-      </c>
+      <c r="J45" s="6"/>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="6"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B46" s="6"/>
@@ -1940,23 +1904,19 @@
       <c r="E46" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="6"/>
+      <c r="F46" s="34">
+        <f>R34</f>
+        <v>4.183561643835616</v>
+      </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
-      <c r="J46" s="34">
-        <f>R34</f>
-        <v>4.183561643835616</v>
-      </c>
+      <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6"/>
-      <c r="S46" s="6"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B47" s="6"/>
@@ -1967,23 +1927,19 @@
       <c r="E47" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="30">
-        <f>J45/(1+J46)^J12</f>
+      <c r="F47" s="30">
+        <f>F45/(1+F46)^F12</f>
         <v>10.921636606380696</v>
       </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
-      <c r="P47" s="6"/>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6"/>
-      <c r="S47" s="6"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B48" s="6"/>
@@ -1994,23 +1950,19 @@
       <c r="E48" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F48" s="6"/>
+      <c r="F48" s="34">
+        <f>$J$37</f>
+        <v>2.9701250363434752</v>
+      </c>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
-      <c r="J48" s="34">
-        <f>$J$37</f>
-        <v>2.9701250363434752</v>
-      </c>
+      <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
-      <c r="P48" s="6"/>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="6"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B49" s="6"/>
@@ -2021,23 +1973,19 @@
       <c r="E49" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="36">
-        <f>SUM(J47:J48)</f>
+      <c r="F49" s="36">
+        <f>SUM(F47:F48)</f>
         <v>13.891761642724171</v>
       </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
-      <c r="S49" s="6"/>
     </row>
     <row r="51" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51"/>

</xml_diff>

<commit_message>
Further modifications to right column
</commit_message>
<xml_diff>
--- a/Assignment/BENDIGO.xlsx
+++ b/Assignment/BENDIGO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh\Documents\GITHUB\FM_equity_research\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A578B6-2DD4-4E88-BF30-5836CC113263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E10344C-81BA-409C-91FB-E525CEB2B20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C40C285E-7926-4BFA-A8EA-1C74888DBDA3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C40C285E-7926-4BFA-A8EA-1C74888DBDA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dividend Discount Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>FY2025</t>
   </si>
@@ -143,12 +143,6 @@
     <t>Valuation Date</t>
   </si>
   <si>
-    <t>Share Price</t>
-  </si>
-  <si>
-    <t>DilutedShares Outstanding</t>
-  </si>
-  <si>
     <t>Cost of Equity</t>
   </si>
   <si>
@@ -167,7 +161,7 @@
     <t>Intrinsic Value</t>
   </si>
   <si>
-    <t>Discount/(Premium)</t>
+    <t>Last Share Price</t>
   </si>
 </sst>
 </file>
@@ -377,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -441,8 +435,10 @@
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -788,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314E70D6-0A07-40D1-BF88-F5CE50014335}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="122" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -801,6 +797,7 @@
     <col min="3" max="3" width="3.1796875" customWidth="1"/>
     <col min="4" max="4" width="44.7265625" customWidth="1"/>
     <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="9.1796875" customWidth="1"/>
     <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="18" width="15.7265625" customWidth="1"/>
@@ -810,7 +807,7 @@
     <row r="2" spans="1:18" s="1" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2"/>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.4">
@@ -927,64 +924,51 @@
     <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="44">
-        <v>45772</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="45">
-        <v>10.88</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9"/>
+      <c r="B9" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+    </row>
+    <row r="10" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="42">
-        <v>566.54</v>
+        <v>34</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="44">
+        <v>45772</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="38"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -997,13 +981,13 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="46">
-        <v>7.9000000000000001E-2</v>
+        <v>15</v>
+      </c>
+      <c r="F12" s="45">
+        <v>10.88</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1019,13 +1003,14 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="31" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="46">
-        <v>2.1000000000000001E-2</v>
+        <v>15</v>
+      </c>
+      <c r="F13" s="45">
+        <f>ROUND(F46,2)</f>
+        <v>13.89</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1040,40 +1025,59 @@
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="42">
+        <v>566.54</v>
+      </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15"/>
-      <c r="B15" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="46">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="D16" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="46">
+        <v>2.1000000000000001E-2</v>
+      </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1081,17 +1085,14 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="22">
-        <f>F10</f>
-        <v>10.88</v>
-      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1101,35 +1102,34 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="34">
-        <f>F49</f>
-        <v>13.891761642724171</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+    <row r="18" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18"/>
+      <c r="B18" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="53">
-        <f>E18/E17-1</f>
-        <v>0.27681632745626561</v>
-      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1138,356 +1138,409 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21"/>
-      <c r="B21" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="40"/>
-      <c r="S21" s="40"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:19" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B21" s="11"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-    </row>
-    <row r="23" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="43">
+        <f>$F$14</f>
+        <v>566.54</v>
+      </c>
+      <c r="L22" s="43">
+        <f>$F$14</f>
+        <v>566.54</v>
+      </c>
+      <c r="M22" s="43">
+        <f>$F$14</f>
+        <v>566.54</v>
+      </c>
+      <c r="N22" s="47">
+        <f>M22</f>
+        <v>566.54</v>
+      </c>
+      <c r="O22" s="16">
+        <f>N22</f>
+        <v>566.54</v>
+      </c>
+      <c r="P22" s="16">
+        <f>O22</f>
+        <v>566.54</v>
+      </c>
+      <c r="Q22" s="16">
+        <f>P22</f>
+        <v>566.54</v>
+      </c>
+      <c r="R22" s="16">
+        <f>Q22</f>
+        <v>566.54</v>
+      </c>
+      <c r="S22" s="7"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B23" s="11"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="42">
+        <v>488.1</v>
+      </c>
+      <c r="L23" s="42">
+        <v>497</v>
+      </c>
+      <c r="M23" s="41">
+        <v>545</v>
+      </c>
+      <c r="N23" s="42">
+        <v>455.86</v>
+      </c>
+      <c r="O23" s="42">
+        <v>491.76</v>
+      </c>
+      <c r="P23" s="42">
+        <v>500.55</v>
+      </c>
+      <c r="Q23" s="42">
+        <v>515.5</v>
+      </c>
+      <c r="R23" s="42">
+        <v>611</v>
+      </c>
+      <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B24" s="11"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="D24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="17">
+        <f>K22*K28</f>
+        <v>300.26619999999997</v>
+      </c>
+      <c r="L24" s="17">
+        <f t="shared" ref="L24:M24" si="0">L22*L28</f>
+        <v>345.58939999999996</v>
+      </c>
+      <c r="M24" s="15">
+        <f t="shared" si="0"/>
+        <v>356.92019999999997</v>
+      </c>
+      <c r="N24" s="17">
+        <f>N28*N22</f>
+        <v>298.65271073691014</v>
+      </c>
+      <c r="O24" s="17">
+        <f t="shared" ref="O24:R24" si="1">O28*O22</f>
+        <v>322.17228322726919</v>
+      </c>
+      <c r="P24" s="17">
+        <f t="shared" si="1"/>
+        <v>327.93097521028471</v>
+      </c>
+      <c r="Q24" s="17">
+        <f t="shared" si="1"/>
+        <v>337.72533757047592</v>
+      </c>
+      <c r="R24" s="17">
+        <f t="shared" si="1"/>
+        <v>400.29133124260096</v>
+      </c>
       <c r="S24" s="7"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>6</v>
-      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="43">
-        <f>$F$11</f>
-        <v>566.54</v>
-      </c>
-      <c r="L25" s="43">
-        <f>$F$11</f>
-        <v>566.54</v>
-      </c>
-      <c r="M25" s="43">
-        <f>$F$11</f>
-        <v>566.54</v>
-      </c>
-      <c r="N25" s="47">
-        <f>M25</f>
-        <v>566.54</v>
-      </c>
-      <c r="O25" s="16">
-        <f>N25</f>
-        <v>566.54</v>
-      </c>
-      <c r="P25" s="16">
-        <f>O25</f>
-        <v>566.54</v>
-      </c>
-      <c r="Q25" s="16">
-        <f>P25</f>
-        <v>566.54</v>
-      </c>
-      <c r="R25" s="16">
-        <f>Q25</f>
-        <v>566.54</v>
-      </c>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
       <c r="S25" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B26" s="11"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="6" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="42">
-        <v>488.1</v>
-      </c>
-      <c r="L26" s="42">
-        <v>497</v>
-      </c>
-      <c r="M26" s="41">
-        <v>545</v>
-      </c>
-      <c r="N26" s="42">
-        <v>455.86</v>
-      </c>
-      <c r="O26" s="42">
-        <v>491.76</v>
-      </c>
-      <c r="P26" s="42">
-        <v>500.55</v>
-      </c>
-      <c r="Q26" s="42">
-        <v>515.5</v>
-      </c>
-      <c r="R26" s="42">
-        <v>611</v>
-      </c>
-      <c r="S26" s="7"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20">
+        <f t="shared" ref="K26:R26" si="2">K23/K22</f>
+        <v>0.86154552194019851</v>
+      </c>
+      <c r="L26" s="20">
+        <f t="shared" si="2"/>
+        <v>0.87725491580470938</v>
+      </c>
+      <c r="M26" s="21">
+        <f t="shared" si="2"/>
+        <v>0.9619797366470153</v>
+      </c>
+      <c r="N26" s="20">
+        <f>N23/N22</f>
+        <v>0.80463868394111637</v>
+      </c>
+      <c r="O26" s="20">
+        <f t="shared" si="2"/>
+        <v>0.86800578952942431</v>
+      </c>
+      <c r="P26" s="20">
+        <f t="shared" si="2"/>
+        <v>0.88352102234617158</v>
+      </c>
+      <c r="Q26" s="20">
+        <f t="shared" si="2"/>
+        <v>0.90990927383768139</v>
+      </c>
+      <c r="R26" s="20">
+        <f t="shared" si="2"/>
+        <v>1.0784763653051859</v>
+      </c>
+      <c r="S26" s="6"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B27" s="11"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="17">
-        <f>K25*K31</f>
-        <v>300.26619999999997</v>
-      </c>
-      <c r="L27" s="17">
-        <f t="shared" ref="L27:M27" si="0">L25*L31</f>
-        <v>345.58939999999996</v>
-      </c>
-      <c r="M27" s="15">
-        <f t="shared" si="0"/>
-        <v>356.92019999999997</v>
-      </c>
-      <c r="N27" s="17">
-        <f>N31*N25</f>
-        <v>298.65271073691014</v>
-      </c>
-      <c r="O27" s="17">
-        <f t="shared" ref="O27:R27" si="1">O31*O25</f>
-        <v>322.17228322726919</v>
-      </c>
-      <c r="P27" s="17">
-        <f t="shared" si="1"/>
-        <v>327.93097521028471</v>
-      </c>
-      <c r="Q27" s="17">
-        <f t="shared" si="1"/>
-        <v>337.72533757047592</v>
-      </c>
-      <c r="R27" s="17">
-        <f t="shared" si="1"/>
-        <v>400.29133124260096</v>
-      </c>
-      <c r="S27" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="50">
+        <f>K24/K23</f>
+        <v>0.61517353001434127</v>
+      </c>
+      <c r="L27" s="50">
+        <f t="shared" ref="L27:M27" si="3">L24/L23</f>
+        <v>0.69535090543259548</v>
+      </c>
+      <c r="M27" s="51">
+        <f t="shared" si="3"/>
+        <v>0.65489944954128432</v>
+      </c>
+      <c r="N27" s="50">
+        <f>AVERAGE($K$27:$M$27)</f>
+        <v>0.65514129499607365</v>
+      </c>
+      <c r="O27" s="50">
+        <f t="shared" ref="O27:R27" si="4">AVERAGE($K$27:$M$27)</f>
+        <v>0.65514129499607365</v>
+      </c>
+      <c r="P27" s="50">
+        <f t="shared" si="4"/>
+        <v>0.65514129499607365</v>
+      </c>
+      <c r="Q27" s="50">
+        <f t="shared" si="4"/>
+        <v>0.65514129499607365</v>
+      </c>
+      <c r="R27" s="50">
+        <f t="shared" si="4"/>
+        <v>0.65514129499607365</v>
+      </c>
+      <c r="S27" s="6"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B28" s="11"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="48">
+        <v>0.53</v>
+      </c>
+      <c r="L28" s="48">
+        <v>0.61</v>
+      </c>
+      <c r="M28" s="49">
+        <v>0.63</v>
+      </c>
+      <c r="N28" s="22">
+        <f>N27*N26</f>
+        <v>0.52715202940111938</v>
+      </c>
+      <c r="O28" s="22">
+        <f t="shared" ref="O28:R28" si="5">O27*O26</f>
+        <v>0.56866643701639641</v>
+      </c>
+      <c r="P28" s="22">
+        <f t="shared" si="5"/>
+        <v>0.57883110673612581</v>
+      </c>
+      <c r="Q28" s="22">
+        <f t="shared" si="5"/>
+        <v>0.59611913999095556</v>
+      </c>
+      <c r="R28" s="22">
+        <f t="shared" si="5"/>
+        <v>0.70655440258869806</v>
+      </c>
+      <c r="S28" s="6"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20">
-        <f t="shared" ref="K29:R29" si="2">K26/K25</f>
-        <v>0.86154552194019851</v>
-      </c>
-      <c r="L29" s="20">
-        <f t="shared" si="2"/>
-        <v>0.87725491580470938</v>
-      </c>
-      <c r="M29" s="21">
-        <f t="shared" si="2"/>
-        <v>0.9619797366470153</v>
-      </c>
-      <c r="N29" s="20">
-        <f>N26/N25</f>
-        <v>0.80463868394111637</v>
-      </c>
-      <c r="O29" s="20">
-        <f t="shared" si="2"/>
-        <v>0.86800578952942431</v>
-      </c>
-      <c r="P29" s="20">
-        <f t="shared" si="2"/>
-        <v>0.88352102234617158</v>
-      </c>
-      <c r="Q29" s="20">
-        <f t="shared" si="2"/>
-        <v>0.90990927383768139</v>
-      </c>
-      <c r="R29" s="20">
-        <f t="shared" si="2"/>
-        <v>1.0784763653051859</v>
-      </c>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
       <c r="S29" s="6"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="50">
-        <f>K27/K26</f>
-        <v>0.61517353001434127</v>
-      </c>
-      <c r="L30" s="50">
-        <f t="shared" ref="L30:M30" si="3">L27/L26</f>
-        <v>0.69535090543259548</v>
-      </c>
-      <c r="M30" s="51">
-        <f t="shared" si="3"/>
-        <v>0.65489944954128432</v>
-      </c>
-      <c r="N30" s="50">
-        <f>AVERAGE($K$30:$M$30)</f>
-        <v>0.65514129499607365</v>
-      </c>
-      <c r="O30" s="50">
-        <f t="shared" ref="O30:R30" si="4">AVERAGE($K$30:$M$30)</f>
-        <v>0.65514129499607365</v>
-      </c>
-      <c r="P30" s="50">
-        <f t="shared" si="4"/>
-        <v>0.65514129499607365</v>
-      </c>
-      <c r="Q30" s="50">
-        <f t="shared" si="4"/>
-        <v>0.65514129499607365</v>
-      </c>
-      <c r="R30" s="50">
-        <f t="shared" si="4"/>
-        <v>0.65514129499607365</v>
+      <c r="J30" s="18"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="23">
+        <f>N5</f>
+        <v>45838</v>
+      </c>
+      <c r="O30" s="23">
+        <f>O5</f>
+        <v>46203</v>
+      </c>
+      <c r="P30" s="23">
+        <f>P5</f>
+        <v>46568</v>
+      </c>
+      <c r="Q30" s="23">
+        <f>Q5</f>
+        <v>46934</v>
+      </c>
+      <c r="R30" s="23">
+        <f>R5</f>
+        <v>47299</v>
       </c>
       <c r="S30" s="6"/>
     </row>
@@ -1495,183 +1548,146 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="48">
-        <v>0.53</v>
-      </c>
-      <c r="L31" s="48">
-        <v>0.61</v>
-      </c>
-      <c r="M31" s="49">
-        <v>0.63</v>
-      </c>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="19"/>
       <c r="N31" s="22">
-        <f>N30*N29</f>
-        <v>0.52715202940111938</v>
+        <f>(N30-$F$11)/365</f>
+        <v>0.18082191780821918</v>
       </c>
       <c r="O31" s="22">
-        <f t="shared" ref="O31:R31" si="5">O30*O29</f>
-        <v>0.56866643701639641</v>
+        <f t="shared" ref="O31:R31" si="6">(O30-$F$11)/365</f>
+        <v>1.1808219178082191</v>
       </c>
       <c r="P31" s="22">
-        <f t="shared" si="5"/>
-        <v>0.57883110673612581</v>
+        <f t="shared" si="6"/>
+        <v>2.1808219178082191</v>
       </c>
       <c r="Q31" s="22">
-        <f t="shared" si="5"/>
-        <v>0.59611913999095556</v>
+        <f t="shared" si="6"/>
+        <v>3.1835616438356165</v>
       </c>
       <c r="R31" s="22">
-        <f t="shared" si="5"/>
-        <v>0.70655440258869806</v>
+        <f t="shared" si="6"/>
+        <v>4.183561643835616</v>
       </c>
       <c r="S31" s="6"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
+      <c r="D32" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="30">
+        <f>N28/(1+F15)^N31</f>
+        <v>0.51995395001129951</v>
+      </c>
+      <c r="O32" s="30">
+        <f>O28/(1+G15)^O31</f>
+        <v>0.56866643701639641</v>
+      </c>
+      <c r="P32" s="30">
+        <f>P28/(1+H15)^P31</f>
+        <v>0.57883110673612581</v>
+      </c>
+      <c r="Q32" s="30">
+        <f>Q28/(1+I15)^Q31</f>
+        <v>0.59611913999095556</v>
+      </c>
+      <c r="R32" s="30">
+        <f>R28/(1+J15)^R31</f>
+        <v>0.70655440258869806</v>
+      </c>
+      <c r="S32" s="27"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="18"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="23">
-        <f>N5</f>
-        <v>45838</v>
-      </c>
-      <c r="O33" s="23">
-        <f t="shared" ref="O33:R33" si="6">O5</f>
-        <v>46203</v>
-      </c>
-      <c r="P33" s="23">
-        <f t="shared" si="6"/>
-        <v>46568</v>
-      </c>
-      <c r="Q33" s="23">
-        <f t="shared" si="6"/>
-        <v>46934</v>
-      </c>
-      <c r="R33" s="23">
-        <f t="shared" si="6"/>
-        <v>47299</v>
-      </c>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
       <c r="S33" s="6"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="6" t="s">
-        <v>21</v>
+      <c r="D34" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="18"/>
+      <c r="J34" s="32">
+        <f>SUM(N32:R32)</f>
+        <v>2.9701250363434752</v>
+      </c>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="19"/>
-      <c r="N34" s="22">
-        <f>(N33-$F$9)/365</f>
-        <v>0.18082191780821918</v>
-      </c>
-      <c r="O34" s="22">
-        <f t="shared" ref="O34:R34" si="7">(O33-$F$9)/365</f>
-        <v>1.1808219178082191</v>
-      </c>
-      <c r="P34" s="22">
-        <f t="shared" si="7"/>
-        <v>2.1808219178082191</v>
-      </c>
-      <c r="Q34" s="22">
-        <f t="shared" si="7"/>
-        <v>3.1835616438356165</v>
-      </c>
-      <c r="R34" s="22">
-        <f t="shared" si="7"/>
-        <v>4.183561643835616</v>
-      </c>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
       <c r="S34" s="6"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="30">
-        <f>N31/(1+F12)^N34</f>
-        <v>0.51995395001129951</v>
-      </c>
-      <c r="O35" s="30">
-        <f>O31/(1+G12)^O34</f>
-        <v>0.56866643701639641</v>
-      </c>
-      <c r="P35" s="30">
-        <f>P31/(1+H12)^P34</f>
-        <v>0.57883110673612581</v>
-      </c>
-      <c r="Q35" s="30">
-        <f>Q31/(1+I12)^Q34</f>
-        <v>0.59611913999095556</v>
-      </c>
-      <c r="R35" s="30">
-        <f>R31/(1+J12)^R34</f>
-        <v>0.70655440258869806</v>
-      </c>
-      <c r="S35" s="27"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B36" s="6"/>
@@ -1682,10 +1698,10 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="19"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="33"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
@@ -1693,32 +1709,28 @@
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="32">
-        <f>SUM(N35:R35)</f>
-        <v>2.9701250363434752</v>
-      </c>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
+      <c r="C37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B38" s="6"/>
@@ -1732,7 +1744,7 @@
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
-      <c r="M38" s="33"/>
+      <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
@@ -1743,52 +1755,62 @@
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="D39" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="34">
+        <f>R28</f>
+        <v>0.70655440258869806</v>
+      </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
-      <c r="M39" s="33"/>
+      <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-    </row>
-    <row r="40" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B40" s="6"/>
-      <c r="C40" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="35">
+        <f>F16</f>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="D41" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="34">
+        <f>F39*(1+F40)</f>
+        <v>0.72139204504306065</v>
+      </c>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -1798,23 +1820,19 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F42" s="34">
-        <f>R31</f>
-        <v>0.70655440258869806</v>
+        <f>F41/(F15-F40)</f>
+        <v>12.437793880052771</v>
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -1830,14 +1848,14 @@
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="35">
-        <f>F13</f>
-        <v>2.1000000000000001E-2</v>
+        <v>22</v>
+      </c>
+      <c r="F43" s="34">
+        <f>R31</f>
+        <v>4.183561643835616</v>
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -1852,15 +1870,15 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" s="13" t="s">
+      <c r="D44" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="34">
-        <f>F42*(1+F43)</f>
-        <v>0.72139204504306065</v>
+      <c r="F44" s="30">
+        <f>F42/(1+F43)^F15</f>
+        <v>10.921636606380696</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -1876,14 +1894,14 @@
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F45" s="34">
-        <f>F44/(F12-F43)</f>
-        <v>12.437793880052771</v>
+        <f>$J$34</f>
+        <v>2.9701250363434752</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -1898,15 +1916,15 @@
     <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="34">
-        <f>R34</f>
-        <v>4.183561643835616</v>
+      <c r="D46" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="36">
+        <f>SUM(F44:F45)</f>
+        <v>13.891761642724171</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -1918,97 +1936,28 @@
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47" s="30">
-        <f>F45/(1+F46)^F12</f>
-        <v>10.921636606380696</v>
-      </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F48" s="34">
-        <f>$J$37</f>
-        <v>2.9701250363434752</v>
-      </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
-      <c r="O48" s="6"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F49" s="36">
-        <f>SUM(F47:F48)</f>
-        <v>13.891761642724171</v>
-      </c>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
-      <c r="M49" s="6"/>
-      <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
-    </row>
-    <row r="51" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51"/>
-      <c r="B51" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="40"/>
-      <c r="N51" s="40"/>
-      <c r="O51" s="40"/>
-      <c r="P51" s="40"/>
-      <c r="Q51" s="40"/>
-      <c r="R51" s="40"/>
-      <c r="S51" s="40"/>
+    <row r="48" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48"/>
+      <c r="B48" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="40"/>
+      <c r="N48" s="40"/>
+      <c r="O48" s="40"/>
+      <c r="P48" s="40"/>
+      <c r="Q48" s="40"/>
+      <c r="R48" s="40"/>
+      <c r="S48" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed formatting and fixed errors in FPDF code
</commit_message>
<xml_diff>
--- a/Assignment/BENDIGO.xlsx
+++ b/Assignment/BENDIGO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d43dd5ddc1e2bd78/Desktop/BAFE/2025 SEM1/FINM3422/Equity Research Assignment/FM_equity_research/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miles\OneDrive\Desktop\BAFE\2025 SEM1\FINM3422\Equity Research Assignment\FM_equity_research\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE4E8A0E-A8CC-4598-A2BE-87CBD8DCB13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AF824D-8083-4A5C-B7F5-0C09E5EFA33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="13403" windowWidth="21795" windowHeight="12975" xr2:uid="{C40C285E-7926-4BFA-A8EA-1C74888DBDA3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{C40C285E-7926-4BFA-A8EA-1C74888DBDA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dividend Discount Model" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>FY2025</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Share Price</t>
-  </si>
-  <si>
-    <t>DilutedShares Outstanding</t>
   </si>
   <si>
     <t>Cost of Equity</t>
@@ -361,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -407,12 +404,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -482,6 +488,10 @@
     <xf numFmtId="168" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -830,7 +840,7 @@
   <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="56" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -849,7 +859,7 @@
     <row r="2" spans="1:19" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2"/>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
@@ -1022,7 +1032,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="31" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>6</v>
@@ -1048,7 +1058,7 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>10</v>
@@ -1114,7 +1124,7 @@
     <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15"/>
       <c r="B15" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="52"/>
       <c r="D15" s="52"/>
@@ -1148,15 +1158,17 @@
       <c r="D17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="22">
-        <f>J10</f>
-        <v>10.88</v>
+      <c r="E17" s="37" t="s">
+        <v>15</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="J17" s="22">
+        <f>J10</f>
+        <v>10.88</v>
+      </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -1165,17 +1177,19 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="34">
+        <v>41</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="22">
         <f>J49</f>
         <v>10.729244797114228</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -1184,17 +1198,19 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="53">
-        <f>E18/E17-1</f>
-        <v>-1.3856176735824621E-2</v>
+        <v>42</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>10</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="J19" s="53">
+        <f>J18/J17-1</f>
+        <v>-1.3856176735824621E-2</v>
+      </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -1507,7 +1523,7 @@
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>10</v>
@@ -2082,7 +2098,7 @@
     <row r="51" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51"/>
       <c r="B51" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
@@ -2126,13 +2142,13 @@
     <row r="2" spans="1:10" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2"/>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3"/>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -2161,40 +2177,40 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="57">
         <v>0.91</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="58">
         <v>4.1399999999999999E-2</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="58">
         <v>0.05</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C12" s="55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="55"/>
       <c r="E12" s="56">

</xml_diff>